<commit_message>
New variations of GA added
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -22,58 +22,58 @@
     <t>E#3</t>
   </si>
   <si>
+    <t>E#11</t>
+  </si>
+  <si>
+    <t>C#0</t>
+  </si>
+  <si>
+    <t>C#1</t>
+  </si>
+  <si>
+    <t>C#2</t>
+  </si>
+  <si>
+    <t>C#3</t>
+  </si>
+  <si>
+    <t>FITNESS</t>
+  </si>
+  <si>
+    <t>PROJECT_#_1</t>
+  </si>
+  <si>
+    <t>E#1</t>
+  </si>
+  <si>
+    <t>E#6</t>
+  </si>
+  <si>
+    <t>PROJECT_#_2</t>
+  </si>
+  <si>
+    <t>E#4</t>
+  </si>
+  <si>
+    <t>E#14</t>
+  </si>
+  <si>
+    <t>PROJECT_#_3</t>
+  </si>
+  <si>
+    <t>E#0</t>
+  </si>
+  <si>
+    <t>E#8</t>
+  </si>
+  <si>
+    <t>PROJECT_#_5</t>
+  </si>
+  <si>
     <t>E#5</t>
   </si>
   <si>
-    <t>C#0</t>
-  </si>
-  <si>
-    <t>C#1</t>
-  </si>
-  <si>
-    <t>C#2</t>
-  </si>
-  <si>
-    <t>C#3</t>
-  </si>
-  <si>
-    <t>FITNESS</t>
-  </si>
-  <si>
-    <t>PROJECT_#_1</t>
-  </si>
-  <si>
-    <t>E#1</t>
-  </si>
-  <si>
-    <t>E#6</t>
-  </si>
-  <si>
-    <t>PROJECT_#_2</t>
-  </si>
-  <si>
-    <t>E#4</t>
-  </si>
-  <si>
-    <t>E#11</t>
-  </si>
-  <si>
-    <t>PROJECT_#_3</t>
-  </si>
-  <si>
-    <t>E#12</t>
-  </si>
-  <si>
-    <t>E#14</t>
-  </si>
-  <si>
-    <t>PROJECT_#_4</t>
-  </si>
-  <si>
-    <t>E#2</t>
-  </si>
-  <si>
-    <t>E#8</t>
+    <t>E#9</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>9.550000000000001</v>
+        <v>8.69</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -471,7 +471,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>8.44</v>
+        <v>12.17</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -479,7 +479,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>9.43</v>
+        <v>13.57</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -487,7 +487,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>10.58</v>
+        <v>11.85</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -495,7 +495,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.3722284915678534</v>
+        <v>0.1498181562069559</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -585,7 +585,7 @@
         <v>3</v>
       </c>
       <c r="B27">
-        <v>9.76</v>
+        <v>9.629999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -593,7 +593,7 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>12.75</v>
+        <v>13.57</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -601,7 +601,7 @@
         <v>5</v>
       </c>
       <c r="B29">
-        <v>14.84</v>
+        <v>12.26</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -609,7 +609,7 @@
         <v>6</v>
       </c>
       <c r="B30">
-        <v>9.149999999999999</v>
+        <v>7.819999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -617,7 +617,7 @@
         <v>7</v>
       </c>
       <c r="B31">
-        <v>0.1284500586631231</v>
+        <v>0.1687855667343836</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -646,7 +646,7 @@
         <v>3</v>
       </c>
       <c r="B38">
-        <v>13.77</v>
+        <v>13.81</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -654,7 +654,7 @@
         <v>4</v>
       </c>
       <c r="B39">
-        <v>8.109999999999999</v>
+        <v>9.67</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -662,7 +662,7 @@
         <v>5</v>
       </c>
       <c r="B40">
-        <v>5.47</v>
+        <v>7.85</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -670,7 +670,7 @@
         <v>6</v>
       </c>
       <c r="B41">
-        <v>9.07</v>
+        <v>9.26</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -678,7 +678,7 @@
         <v>7</v>
       </c>
       <c r="B42">
-        <v>0.1530498306376764</v>
+        <v>0.1177570439251672</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -707,7 +707,7 @@
         <v>3</v>
       </c>
       <c r="B49">
-        <v>10.29</v>
+        <v>8.24</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -715,7 +715,7 @@
         <v>4</v>
       </c>
       <c r="B50">
-        <v>8.140000000000001</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -723,7 +723,7 @@
         <v>5</v>
       </c>
       <c r="B51">
-        <v>3.44</v>
+        <v>5.59</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -731,7 +731,7 @@
         <v>6</v>
       </c>
       <c r="B52">
-        <v>11.15</v>
+        <v>3.74</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -739,7 +739,7 @@
         <v>7</v>
       </c>
       <c r="B53">
-        <v>0.2130081278849053</v>
+        <v>0.2640434866848801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>